<commit_message>
Actualizo proyecto: dashboard, Excel y nuevas imágenes
</commit_message>
<xml_diff>
--- a/Proyecto Analisis financiero.xlsx
+++ b/Proyecto Analisis financiero.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\Proyecto analisis financiero\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\Github\proyecto_analisis_financiero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC3358E-295E-4039-B822-9494C1EB1F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4ADF55C-2602-4940-B254-6E310F4180ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1072,7 +1072,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1416,7 +1416,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -1424,6 +1423,15 @@
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="24">
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1435,15 +1443,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -21150,7 +21149,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="es-AR" sz="2400" b="0"/>
-            <a:t>“Dashboard Financiero – Desempeño Operativo y Estructura”</a:t>
+            <a:t>Dashboard Financiero – Desempeño Operativo y Estructura</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -22348,8 +22347,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{61435D2A-6578-4661-85CF-DE714BE081C4}" name="utilidadnetaTD" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="632">
-  <location ref="A8:B12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CAE8F753-38DB-46F8-ADAE-F74BE07874D2}" name="ROA-ROE" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+  <location ref="G27:I31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
       <items count="4">
@@ -22360,14 +22359,311 @@
       </items>
     </pivotField>
     <pivotField axis="axisCol" showAll="0">
-      <items count="4">
+      <items count="9">
+        <item h="1" x="7"/>
+        <item h="1" x="6"/>
         <item h="1" x="1"/>
         <item h="1" x="0"/>
+        <item h="1" x="5"/>
+        <item h="1" x="4"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de Valor" fld="2" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="4">
+    <chartFormat chart="2" format="20" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="21" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="8" format="24" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="8" format="25" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D448FDD9-3538-4A18-932B-F8D4BA4E4D31}" name="TablaDinámica10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="253">
+  <location ref="W2:Y7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
         <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" numFmtId="168" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de Monto" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="10">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="251" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="252" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{11FFE9A6-3ED4-473D-9617-7D7EC5A43C85}" name="CapitalcontableTD" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="340">
+  <location ref="R2:S6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="6">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item x="4"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
@@ -22394,12 +22690,7 @@
   <dataFields count="1">
     <dataField name="Suma de Monto" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
-  <formats count="1">
-    <format dxfId="0">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="4">
+  <chartFormats count="8">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -22409,25 +22700,79 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="0" series="1">
+    <chartFormat chart="0" format="1" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="630" format="2" series="1">
+    <chartFormat chart="0" format="4" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="631" format="1" series="1">
+    <chartFormat chart="338" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="339" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="338" format="7" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -22449,7 +22794,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F29F14FC-8BB5-4FE0-93AE-8DD09D10CF7C}" name="RatiosrentabilidadTD" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="666">
   <location ref="G2:I6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
@@ -22505,7 +22850,7 @@
     <dataField name="Suma de Valor" fld="2" baseField="0" baseItem="0" numFmtId="10"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="6">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -22667,7 +23012,395 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8E8F34DA-C2F1-4F03-B386-A2388196E6DC}" name="RatiooperacionTD" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="394">
+  <location ref="G21:I24" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="2" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de Valor" fld="2" baseField="0" baseItem="0" numFmtId="2"/>
+  </dataFields>
+  <chartFormats count="7">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="391" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="391" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="393" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="393" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="391" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{541708B4-728A-4F60-ACDB-0BF5BAE592CD}" name="RatiosliquidezTD" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="389">
+  <location ref="G8:I12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="9">
+        <item h="1" x="7"/>
+        <item h="1" x="6"/>
+        <item h="1" x="1"/>
+        <item h="1" x="0"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de Valor" fld="2" baseField="0" baseItem="0" numFmtId="2"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="2">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="6">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="386" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="386" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="388" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="388" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{61435D2A-6578-4661-85CF-DE714BE081C4}" name="utilidadnetaTD" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="632">
+  <location ref="A8:B12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item h="1" x="1"/>
+        <item h="1" x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="168" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="1">
+    <i>
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma de Monto" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="3">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="630" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="631" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1D3A61D2-7D61-47D0-B129-4B06E7D8F6A3}" name="estadosderesultadosTD" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="603">
   <location ref="A2:D6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
@@ -22721,14 +23454,14 @@
     <dataField name="Promedio de Monto" fld="2" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="2">
+    <format dxfId="5">
       <pivotArea field="0" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="4">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -22917,592 +23650,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A2F02939-9885-4A25-A07B-B7C839E2FD5E}" name="RatiosolvenciaTD" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="326">
-  <location ref="G14:I18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="9">
-        <item x="7"/>
-        <item x="6"/>
-        <item h="1" x="1"/>
-        <item h="1" x="0"/>
-        <item h="1" x="5"/>
-        <item h="1" x="4"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Suma de Valor" fld="2" baseField="0" baseItem="0" numFmtId="2"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="3">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="6">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="323" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="323" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="325" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="325" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{11FFE9A6-3ED4-473D-9617-7D7EC5A43C85}" name="CapitalcontableTD" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="340">
-  <location ref="R2:S6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="6">
-        <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item x="4"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="1">
-    <i>
-      <x v="2"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Suma de Monto" fld="2" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="8">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="338" format="6" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="339" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="338" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8E8F34DA-C2F1-4F03-B386-A2388196E6DC}" name="RatiooperacionTD" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="394">
-  <location ref="G21:I24" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="3">
-        <item x="0"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="2" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Suma de Valor" fld="2" baseField="0" baseItem="0" numFmtId="2"/>
-  </dataFields>
-  <chartFormats count="7">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="391" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="391" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="393" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="393" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="391" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{541708B4-728A-4F60-ACDB-0BF5BAE592CD}" name="RatiosliquidezTD" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="389">
-  <location ref="G8:I12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="9">
-        <item h="1" x="7"/>
-        <item h="1" x="6"/>
-        <item h="1" x="1"/>
-        <item h="1" x="0"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Suma de Valor" fld="2" baseField="0" baseItem="0" numFmtId="2"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="4">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="6">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="386" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="386" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="388" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="388" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C5DD575E-4A17-4CB0-AFAC-39E8D4BFFA11}" name="BalanceTD" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="239">
   <location ref="M2:P8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
@@ -23901,182 +24049,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D448FDD9-3538-4A18-932B-F8D4BA4E4D31}" name="TablaDinámica10" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="253">
-  <location ref="W2:Y7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="3">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="2">
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Suma de Monto" fld="2" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="10">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="6" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="251" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="252" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CAE8F753-38DB-46F8-ADAE-F74BE07874D2}" name="ROA-ROE" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
-  <location ref="G27:I31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A2F02939-9885-4A25-A07B-B7C839E2FD5E}" name="RatiosolvenciaTD" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="326">
+  <location ref="G14:I18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
       <items count="4">
@@ -24088,14 +24063,14 @@
     </pivotField>
     <pivotField axis="axisCol" showAll="0">
       <items count="9">
-        <item h="1" x="7"/>
-        <item h="1" x="6"/>
+        <item x="7"/>
+        <item x="6"/>
         <item h="1" x="1"/>
         <item h="1" x="0"/>
         <item h="1" x="5"/>
         <item h="1" x="4"/>
-        <item x="2"/>
-        <item x="3"/>
+        <item h="1" x="2"/>
+        <item h="1" x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -24120,65 +24095,89 @@
   </colFields>
   <colItems count="2">
     <i>
-      <x v="6"/>
+      <x/>
     </i>
     <i>
-      <x v="7"/>
+      <x v="1"/>
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Suma de Valor" fld="2" baseField="0" baseItem="0" numFmtId="10"/>
+    <dataField name="Suma de Valor" fld="2" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="5">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
-  <chartFormats count="4">
-    <chartFormat chart="2" format="20" series="1">
+  <chartFormats count="6">
+    <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="1" count="1" selected="0">
-            <x v="6"/>
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="21" series="1">
+    <chartFormat chart="0" format="1" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="1" count="1" selected="0">
-            <x v="7"/>
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="8" format="24" series="1">
+    <chartFormat chart="323" format="8" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="1" count="1" selected="0">
-            <x v="6"/>
+            <x v="0"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="8" format="25" series="1">
+    <chartFormat chart="323" format="9" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="1" count="1" selected="0">
-            <x v="7"/>
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="325" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="325" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -24289,8 +24288,8 @@
 <file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
   <slicer name="Año" xr10:uid="{6698F1A9-01B5-4DB6-B57F-FDC4BA4FC225}" cache="SegmentaciónDeDatos_Año" caption="Estado de resultado Años" columnCount="3" rowHeight="241300"/>
-  <slicer name="Tipo" xr10:uid="{F657E66C-0D6D-47A9-830D-03ABC973E5BF}" cache="SegmentaciónDeDatos_Tipo" caption="Tipo" rowHeight="241300"/>
-  <slicer name="Tipo 1" xr10:uid="{DDE71A3A-2A0E-4305-8762-12958D6BCF6C}" cache="SegmentaciónDeDatos_Tipo1" caption="Tipo" rowHeight="241300"/>
+  <slicer name="Tipo" xr10:uid="{F657E66C-0D6D-47A9-830D-03ABC973E5BF}" cache="SegmentaciónDeDatos_Tipo" caption="Estado de resultados" rowHeight="241300"/>
+  <slicer name="Tipo 1" xr10:uid="{DDE71A3A-2A0E-4305-8762-12958D6BCF6C}" cache="SegmentaciónDeDatos_Tipo1" caption="Balance" rowHeight="241300"/>
   <slicer name="Año 1" xr10:uid="{2E65C332-F204-41FE-9EAC-4D3660134D5F}" cache="SegmentaciónDeDatos_Año1" caption="Balance Años" columnCount="3" rowHeight="241300"/>
 </slicers>
 </file>
@@ -31230,13 +31229,13 @@
       <c r="M4" s="128" t="s">
         <v>128</v>
       </c>
-      <c r="N4" s="153">
+      <c r="N4">
         <v>855</v>
       </c>
-      <c r="O4" s="153">
+      <c r="O4">
         <v>1083</v>
       </c>
-      <c r="P4" s="153">
+      <c r="P4">
         <v>1515</v>
       </c>
       <c r="R4" s="128">
@@ -31280,13 +31279,13 @@
       <c r="M5" s="128" t="s">
         <v>135</v>
       </c>
-      <c r="N5" s="153">
+      <c r="N5">
         <v>967</v>
       </c>
-      <c r="O5" s="153">
+      <c r="O5">
         <v>990</v>
       </c>
-      <c r="P5" s="153">
+      <c r="P5">
         <v>950</v>
       </c>
       <c r="R5" s="128">
@@ -31330,13 +31329,13 @@
       <c r="M6" s="128" t="s">
         <v>142</v>
       </c>
-      <c r="N6" s="153">
+      <c r="N6">
         <v>743</v>
       </c>
-      <c r="O6" s="153">
+      <c r="O6">
         <v>971</v>
       </c>
-      <c r="P6" s="153">
+      <c r="P6">
         <v>1285</v>
       </c>
       <c r="R6" s="128">
@@ -31359,13 +31358,13 @@
       <c r="M7" s="128" t="s">
         <v>138</v>
       </c>
-      <c r="N7" s="153">
+      <c r="N7">
         <v>576</v>
       </c>
-      <c r="O7" s="153">
+      <c r="O7">
         <v>548</v>
       </c>
-      <c r="P7" s="153">
+      <c r="P7">
         <v>640</v>
       </c>
       <c r="W7" s="128" t="s">
@@ -31394,13 +31393,13 @@
       <c r="M8" s="128" t="s">
         <v>140</v>
       </c>
-      <c r="N8" s="153">
+      <c r="N8">
         <v>534</v>
       </c>
-      <c r="O8" s="153">
+      <c r="O8">
         <v>554</v>
       </c>
-      <c r="P8" s="153">
+      <c r="P8">
         <v>540</v>
       </c>
     </row>
@@ -31627,7 +31626,7 @@
   <dimension ref="A1:AA41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>